<commit_message>
correct add Rwanda and change input file structure
</commit_message>
<xml_diff>
--- a/data/XLSX/risk_factors.xlsx
+++ b/data/XLSX/risk_factors.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unfao-my.sharepoint.com/personal/luc_warde_fao_org/Documents/Document/Shinyapp/esf-shiny-DALYs/data/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="8_{DB7C2F86-2D12-40F4-AB04-F2DE522950B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{57178022-3F11-7341-BD15-71851A2B3DDD}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="8_{DB7C2F86-2D12-40F4-AB04-F2DE522950B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FAC1A0FF-9763-B643-94FF-C9AD6BECD013}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="680" windowWidth="30240" windowHeight="18960" xr2:uid="{35B382DE-C4F0-4686-87E5-67BB7E946CBA}"/>
   </bookViews>
@@ -20,10 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="38">
-  <si>
-    <t>country</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="35">
   <si>
     <t>factor_type</t>
   </si>
@@ -37,9 +34,6 @@
     <t>weight</t>
   </si>
   <si>
-    <t>Zimbabwe</t>
-  </si>
-  <si>
     <t>inherent</t>
   </si>
   <si>
@@ -131,9 +125,6 @@
   </si>
   <si>
     <t>Was this business linked in the past 3 years to a documented food safety related outbreak?</t>
-  </si>
-  <si>
-    <t>Rwanda</t>
   </si>
 </sst>
 </file>
@@ -994,15 +985,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D2ECEAA-4B47-4742-BD0C-3F8D92BEF3D7}">
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1015,483 +1006,200 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
+      <c r="C3" t="s">
         <v>8</v>
       </c>
-      <c r="E2">
+      <c r="D3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" t="s">
-        <v>19</v>
-      </c>
-      <c r="E7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" t="s">
-        <v>21</v>
-      </c>
-      <c r="E8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" t="s">
-        <v>23</v>
-      </c>
-      <c r="E9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10" t="s">
-        <v>25</v>
-      </c>
-      <c r="E10">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" t="s">
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>26</v>
       </c>
-      <c r="D11" t="s">
-        <v>27</v>
-      </c>
-      <c r="E11">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>5</v>
-      </c>
-      <c r="B12" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12" t="s">
-        <v>29</v>
-      </c>
-      <c r="D12" t="s">
-        <v>30</v>
-      </c>
-      <c r="E12">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>5</v>
-      </c>
-      <c r="B13" t="s">
-        <v>28</v>
-      </c>
-      <c r="C13" t="s">
-        <v>31</v>
-      </c>
-      <c r="D13" t="s">
-        <v>32</v>
-      </c>
-      <c r="E13">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>5</v>
-      </c>
-      <c r="B14" t="s">
-        <v>28</v>
-      </c>
-      <c r="C14" t="s">
+      <c r="B15" t="s">
         <v>33</v>
       </c>
-      <c r="D14" t="s">
+      <c r="C15" t="s">
         <v>34</v>
       </c>
-      <c r="E14">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>5</v>
-      </c>
-      <c r="B15" t="s">
-        <v>28</v>
-      </c>
-      <c r="C15" t="s">
-        <v>35</v>
-      </c>
-      <c r="D15" t="s">
-        <v>36</v>
-      </c>
-      <c r="E15">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>37</v>
-      </c>
-      <c r="B16" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16" t="s">
-        <v>7</v>
-      </c>
-      <c r="D16" t="s">
-        <v>8</v>
-      </c>
-      <c r="E16">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>37</v>
-      </c>
-      <c r="B17" t="s">
-        <v>6</v>
-      </c>
-      <c r="C17" t="s">
-        <v>9</v>
-      </c>
-      <c r="D17" t="s">
-        <v>10</v>
-      </c>
-      <c r="E17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>37</v>
-      </c>
-      <c r="B18" t="s">
-        <v>11</v>
-      </c>
-      <c r="C18" t="s">
-        <v>12</v>
-      </c>
-      <c r="D18" t="s">
-        <v>13</v>
-      </c>
-      <c r="E18">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>37</v>
-      </c>
-      <c r="B19" t="s">
-        <v>11</v>
-      </c>
-      <c r="C19" t="s">
-        <v>14</v>
-      </c>
-      <c r="D19" t="s">
-        <v>15</v>
-      </c>
-      <c r="E19">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>37</v>
-      </c>
-      <c r="B20" t="s">
-        <v>11</v>
-      </c>
-      <c r="C20" t="s">
-        <v>16</v>
-      </c>
-      <c r="D20" t="s">
-        <v>17</v>
-      </c>
-      <c r="E20">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>37</v>
-      </c>
-      <c r="B21" t="s">
-        <v>11</v>
-      </c>
-      <c r="C21" t="s">
-        <v>18</v>
-      </c>
-      <c r="D21" t="s">
-        <v>19</v>
-      </c>
-      <c r="E21">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>37</v>
-      </c>
-      <c r="B22" t="s">
-        <v>11</v>
-      </c>
-      <c r="C22" t="s">
-        <v>20</v>
-      </c>
-      <c r="D22" t="s">
-        <v>21</v>
-      </c>
-      <c r="E22">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>37</v>
-      </c>
-      <c r="B23" t="s">
-        <v>11</v>
-      </c>
-      <c r="C23" t="s">
-        <v>22</v>
-      </c>
-      <c r="D23" t="s">
-        <v>23</v>
-      </c>
-      <c r="E23">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>37</v>
-      </c>
-      <c r="B24" t="s">
-        <v>11</v>
-      </c>
-      <c r="C24" t="s">
-        <v>24</v>
-      </c>
-      <c r="D24" t="s">
-        <v>25</v>
-      </c>
-      <c r="E24">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>37</v>
-      </c>
-      <c r="B25" t="s">
-        <v>11</v>
-      </c>
-      <c r="C25" t="s">
-        <v>26</v>
-      </c>
-      <c r="D25" t="s">
-        <v>27</v>
-      </c>
-      <c r="E25">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>37</v>
-      </c>
-      <c r="B26" t="s">
-        <v>28</v>
-      </c>
-      <c r="C26" t="s">
-        <v>29</v>
-      </c>
-      <c r="D26" t="s">
-        <v>30</v>
-      </c>
-      <c r="E26">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>37</v>
-      </c>
-      <c r="B27" t="s">
-        <v>28</v>
-      </c>
-      <c r="C27" t="s">
-        <v>31</v>
-      </c>
-      <c r="D27" t="s">
-        <v>32</v>
-      </c>
-      <c r="E27">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>37</v>
-      </c>
-      <c r="B28" t="s">
-        <v>28</v>
-      </c>
-      <c r="C28" t="s">
-        <v>33</v>
-      </c>
-      <c r="D28" t="s">
-        <v>34</v>
-      </c>
-      <c r="E28">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>37</v>
-      </c>
-      <c r="B29" t="s">
-        <v>28</v>
-      </c>
-      <c r="C29" t="s">
-        <v>35</v>
-      </c>
-      <c r="D29" t="s">
-        <v>36</v>
-      </c>
-      <c r="E29">
+      <c r="D15">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Modified product types labels in script and and factors questions labels in risk factors excel file
</commit_message>
<xml_diff>
--- a/data/XLSX/risk_factors.xlsx
+++ b/data/XLSX/risk_factors.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unfao-my.sharepoint.com/personal/luc_warde_fao_org/Documents/Document/Shinyapp/esf-shiny-DALYs/data/xlsx/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unfao-my.sharepoint.com/personal/stefano_dicandia_fao_org/Documents/Documenti/esf-shiny-DALYs/data/XLSX/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="8_{DB7C2F86-2D12-40F4-AB04-F2DE522950B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FAC1A0FF-9763-B643-94FF-C9AD6BECD013}"/>
+  <xr:revisionPtr revIDLastSave="28" documentId="8_{DB7C2F86-2D12-40F4-AB04-F2DE522950B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F2775CF6-9B2D-4F65-BDFD-0F9226B59FA0}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="680" windowWidth="30240" windowHeight="18960" xr2:uid="{35B382DE-C4F0-4686-87E5-67BB7E946CBA}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{35B382DE-C4F0-4686-87E5-67BB7E946CBA}"/>
   </bookViews>
   <sheets>
     <sheet name="risk_factors" sheetId="1" r:id="rId1"/>
@@ -40,91 +40,91 @@
     <t>vulnerable_distribution</t>
   </si>
   <si>
-    <t>Direct distribution to a vulnerable population (e.g. distribution in hospital, elderly facilities, baby care unit, ...)</t>
-  </si>
-  <si>
     <t>vulnerable_food</t>
   </si>
   <si>
-    <t>Food made for a vulnerable population (such as Baby Food)</t>
-  </si>
-  <si>
     <t>mitigation</t>
   </si>
   <si>
     <t>certification</t>
   </si>
   <si>
-    <t>Certification of the business food safety control system: Accreditation of the food safety control system (e.g. HACCP, ISO 22000, ...) by a reputable body</t>
-  </si>
-  <si>
     <t>training</t>
   </si>
   <si>
-    <t>An adequate Food Safety Training program (e.g. PAHO Food Handlers Manual) for employees (manipulating/processing food) is in place</t>
-  </si>
-  <si>
     <t>export_recognition</t>
   </si>
   <si>
-    <t>Recognition of the business by a relevant authority to export products to other countries</t>
-  </si>
-  <si>
     <t>potable_water</t>
   </si>
   <si>
-    <t>Access to potable water, as demonstrated by annual on site test results or by municipal authorities</t>
-  </si>
-  <si>
     <t>sanitary_facilities</t>
   </si>
   <si>
-    <t>Presence of and access by the personnel of functional and adequately maintained sanitary facilities (e.g. toilets)</t>
-  </si>
-  <si>
     <t>handwashing_facilities</t>
   </si>
   <si>
-    <t>Access by the personnel to functional and adequately maintained hand washing facilities</t>
-  </si>
-  <si>
     <t>electrical_power</t>
   </si>
   <si>
-    <t>Presence and continuous access to electrical power</t>
-  </si>
-  <si>
     <t>cooling_equipment</t>
   </si>
   <si>
-    <t>Presence and continuous access of sufficient cooling equipments according to the expected need (e.g. adequate cooling system if the product needs to be cool)</t>
-  </si>
-  <si>
     <t>compliance</t>
   </si>
   <si>
     <t>current_nonconformity</t>
   </si>
   <si>
-    <t>Inspection results. Presence of at least one important non-conformity in the current visit directly linked to food safety</t>
-  </si>
-  <si>
     <t>past_nonconformity</t>
   </si>
   <si>
-    <t>Inspection results. Presence of at least one important non-conformity in the last visit directly linked to food safety</t>
-  </si>
-  <si>
     <t>enforcement_history</t>
   </si>
   <si>
-    <t>History of enforcement actions in the past 5 years: was this business targeted by an enforcement action such as permit suspension or temporary cessation of activities by inspection authorities</t>
-  </si>
-  <si>
     <t>outbreak_linked</t>
   </si>
   <si>
-    <t>Was this business linked in the past 3 years to a documented food safety related outbreak?</t>
+    <t>Direct distribution to vulnerable populations (e.g., hospitals, elderly care facilities, neonatal units)</t>
+  </si>
+  <si>
+    <t>Food specifically intended for vulnerable populations (e.g., infant formula, meals for elderly individuals)</t>
+  </si>
+  <si>
+    <t>Certification or accreditation of the business food safety management system (e.g. HACCP, ISO 22000) by a reputable body</t>
+  </si>
+  <si>
+    <t>Adequate food safety training for employees (e.g., PAHO Food Handlers Manual), especially those handling or processing food</t>
+  </si>
+  <si>
+    <t>Official recognition by competent authorities for export eligibility</t>
+  </si>
+  <si>
+    <t>Verified access to potable water (e.g., annual on-site tests or municipal certification)</t>
+  </si>
+  <si>
+    <t>Functional and well-maintained sanitary facilities available for personnel (e.g., toilets)</t>
+  </si>
+  <si>
+    <t>Functional and well-maintained handwashing facilities accessible to personnel</t>
+  </si>
+  <si>
+    <t>Reliable and continuous access to electrical power</t>
+  </si>
+  <si>
+    <t>Adequate and continuously available cooling equipment based on product requirements (e.g., refrigeration for perishable goods)</t>
+  </si>
+  <si>
+    <t>Current inspection identified at least one major food safety non-conformity</t>
+  </si>
+  <si>
+    <t>The food business has faced enforcement actions by inspection authorities within the past 5 years (e.g., permit suspension, temporary closure)</t>
+  </si>
+  <si>
+    <t>Previous inspection identified at least one major food safety non-conformity</t>
+  </si>
+  <si>
+    <t>Food business linked to a documented foodborne outbreak within the past 3 years</t>
   </si>
 </sst>
 </file>
@@ -987,13 +987,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D2ECEAA-4B47-4742-BD0C-3F8D92BEF3D7}">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="155.109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1007,7 +1012,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1015,186 +1020,186 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="D2">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="D3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="D4">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
         <v>9</v>
       </c>
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="D5">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="D6">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="D7">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="D8">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="D9">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C10" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="D10">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="C11" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D11">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="C12" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D12">
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="B13" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="C13" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D13">
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="B14" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="C14" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D14">
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="B15" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="C15" t="s">
         <v>34</v>

</xml_diff>

<commit_message>
Update risk factor weight for previous inspection from 5 to 4 and history from 4 to 5
</commit_message>
<xml_diff>
--- a/data/XLSX/risk_factors.xlsx
+++ b/data/XLSX/risk_factors.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11130"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unfao-my.sharepoint.com/personal/stefano_dicandia_fao_org/Documents/Documenti/esf-shiny-DALYs/data/XLSX/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unfao-my.sharepoint.com/personal/luc_warde_fao_org/Documents/Document/Shinyapp/esf-shiny-DALYs/data/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="28" documentId="8_{DB7C2F86-2D12-40F4-AB04-F2DE522950B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F2775CF6-9B2D-4F65-BDFD-0F9226B59FA0}"/>
+  <xr:revisionPtr revIDLastSave="33" documentId="8_{DB7C2F86-2D12-40F4-AB04-F2DE522950B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5A1271EA-969D-EB43-A3F4-47B2B850BF94}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{35B382DE-C4F0-4686-87E5-67BB7E946CBA}"/>
+    <workbookView xWindow="2740" yWindow="-21600" windowWidth="38400" windowHeight="21600" xr2:uid="{35B382DE-C4F0-4686-87E5-67BB7E946CBA}"/>
   </bookViews>
   <sheets>
     <sheet name="risk_factors" sheetId="1" r:id="rId1"/>
@@ -987,18 +987,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D2ECEAA-4B47-4742-BD0C-3F8D92BEF3D7}">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="155.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="117.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1012,7 +1012,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1026,7 +1026,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1040,7 +1040,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -1054,7 +1054,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -1068,7 +1068,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -1082,7 +1082,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1096,7 +1096,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1110,7 +1110,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1124,7 +1124,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -1138,7 +1138,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -1152,7 +1152,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -1166,7 +1166,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -1177,10 +1177,10 @@
         <v>32</v>
       </c>
       <c r="D13">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -1191,10 +1191,10 @@
         <v>33</v>
       </c>
       <c r="D14">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>16</v>
       </c>

</xml_diff>